<commit_message>
Add full diff key genes 1000 iterations results
</commit_message>
<xml_diff>
--- a/results/humanPVATsn/pathfindR/comparison1v3/mature_healthy_vs_obese_excel.xlsx
+++ b/results/humanPVATsn/pathfindR/comparison1v3/mature_healthy_vs_obese_excel.xlsx
@@ -1,26 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahbazin/Desktop/Cambridge/Academics/Han_Lab/MPhil/mphil-project/results/humanPVATsn/pathfindR/comparison1v3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{9E09FA27-500B-4C47-BAED-26E8B15C24E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{945D2D5A-3661-CF42-9C25-4605232DDD98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15680" xr2:uid="{0429090D-58E2-D145-AA28-FEBA789750A7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{0429090D-58E2-D145-AA28-FEBA789750A7}"/>
   </bookViews>
   <sheets>
     <sheet name="mature_healthy_vs_obese" sheetId="1" r:id="rId1"/>
+    <sheet name="healthy only" sheetId="2" r:id="rId2"/>
+    <sheet name="obese only" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">mature_healthy_vs_obese!$L$1:$L$342</definedName>
+  </definedNames>
   <calcPr calcId="0" refMode="R1C1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3541" uniqueCount="1624">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3740" uniqueCount="1624">
   <si>
     <t>ID</t>
   </si>
@@ -4898,7 +4903,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -5033,8 +5038,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="37">
+  <fills count="42">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5238,6 +5264,36 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCAEDFB"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF40FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -5399,16 +5455,26 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -5458,6 +5524,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF40FF"/>
       <color rgb="FFFF2F92"/>
       <color rgb="FF00FDFF"/>
     </mruColors>
@@ -5792,41 +5859,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBFC56C5-C647-6A40-AEAE-C422E355FC30}">
   <dimension ref="A1:S342"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D244" sqref="D244"/>
+    <sheetView zoomScale="87" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="46.33203125" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="11" max="11" width="20.83203125" customWidth="1"/>
+    <col min="12" max="12" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
+      <c r="A1" s="8"/>
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="8" t="s">
         <v>8</v>
       </c>
       <c r="K1" t="s">
@@ -5858,33 +5929,34 @@
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A2">
+      <c r="A2" s="8">
         <v>38</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="8">
         <v>11.071125611745501</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="8">
         <v>9</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="8">
         <v>0.01</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="8">
         <v>1.6992237622300199E-3</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="8">
         <v>2.2210984765881299E-2</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="8" t="s">
         <v>208</v>
       </c>
+      <c r="J2" s="8"/>
       <c r="K2" t="s">
         <v>29</v>
       </c>
@@ -5970,34 +6042,34 @@
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="A4" s="8">
         <v>338</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="8" t="s">
         <v>1603</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="8" t="s">
         <v>1604</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="8">
         <v>10.543929154043299</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="8">
         <v>10</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="8">
         <v>7.4999999999999997E-3</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="8">
         <v>7.0301221975595197E-4</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="8">
         <v>3.6002885332356502E-2</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="8" t="s">
         <v>1605</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="8" t="s">
         <v>1606</v>
       </c>
       <c r="K4" t="s">
@@ -6029,33 +6101,34 @@
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="A5" s="8">
         <v>39</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="8">
         <v>9.2259380097879298</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="8">
         <v>7</v>
       </c>
-      <c r="F5">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="G5">
+      <c r="F5" s="8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G5" s="8">
         <v>3.3893226242257498E-3</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="8">
         <v>4.4136445464832703E-2</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="8" t="s">
         <v>208</v>
       </c>
+      <c r="J5" s="8"/>
       <c r="K5" t="s">
         <v>29</v>
       </c>
@@ -6141,34 +6214,34 @@
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="A7" s="8">
         <v>227</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="8" t="s">
         <v>1112</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="8" t="s">
         <v>1113</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="8">
         <v>9.2259380097879298</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="8">
         <v>10</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="8">
         <v>0.01</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="8">
         <v>8.8380266195254593E-3</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="8">
         <v>1.01548233492488E-2</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="8" t="s">
         <v>1114</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="8" t="s">
         <v>1115</v>
       </c>
       <c r="K7" t="s">
@@ -6200,34 +6273,34 @@
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A8">
+      <c r="A8" s="8">
         <v>162</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="8" t="s">
         <v>810</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="8" t="s">
         <v>811</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="8">
         <v>8.2008337864781602</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="8">
         <v>10</v>
       </c>
-      <c r="F8">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="G8">
+      <c r="F8" s="8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G8" s="8">
         <v>2.5354327311328199E-2</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="8">
         <v>3.3589083428184202E-2</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="8" t="s">
         <v>812</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="8" t="s">
         <v>813</v>
       </c>
       <c r="K8" t="s">
@@ -6259,33 +6332,34 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="A9" s="8">
         <v>89</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="8" t="s">
         <v>487</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="8" t="s">
         <v>488</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="8">
         <v>7.9079468655325096</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="8">
         <v>10</v>
       </c>
-      <c r="F9">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="G9">
+      <c r="F9" s="8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G9" s="8">
         <v>5.9153911943800597E-3</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="8">
         <v>6.3517506854606698E-3</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="8" t="s">
         <v>489</v>
       </c>
+      <c r="J9" s="8"/>
       <c r="K9" t="s">
         <v>29</v>
       </c>
@@ -6315,31 +6389,32 @@
       </c>
     </row>
     <row r="10" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
+      <c r="A10" s="8">
         <v>95</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="8" t="s">
         <v>509</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="8" t="s">
         <v>510</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="8">
         <v>7.9079468655325096</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="8">
         <v>9</v>
       </c>
-      <c r="F10" s="2">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="G10" s="2">
+      <c r="F10" s="8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G10" s="8">
         <v>1.06339454561624E-2</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10" s="8">
         <v>4.5148842306685699E-2</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="I10" s="8"/>
+      <c r="J10" s="8" t="s">
         <v>511</v>
       </c>
       <c r="K10" s="2" t="s">
@@ -6430,31 +6505,32 @@
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A12">
+      <c r="A12" s="8">
         <v>75</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="8" t="s">
         <v>412</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="8" t="s">
         <v>413</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="8">
         <v>6.9194535073409504</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="8">
         <v>10</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="8">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="8">
         <v>5.9774090505759899E-4</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="8">
         <v>2.0743455891261602E-3</v>
       </c>
-      <c r="J12" t="s">
+      <c r="I12" s="8"/>
+      <c r="J12" s="8" t="s">
         <v>414</v>
       </c>
       <c r="K12" t="s">
@@ -6486,34 +6562,34 @@
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A13">
+      <c r="A13" s="8">
         <v>124</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="8" t="s">
         <v>635</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="8" t="s">
         <v>636</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="8">
         <v>6.9194535073409504</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="8">
         <v>10</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="8">
         <v>7.4999999999999997E-3</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="8">
         <v>1.5499421234584299E-2</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="8">
         <v>1.7464354312875598E-2</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I13" s="8" t="s">
         <v>637</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" s="8" t="s">
         <v>638</v>
       </c>
       <c r="K13" t="s">
@@ -6545,34 +6621,34 @@
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A14">
+      <c r="A14" s="8">
         <v>336</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="8" t="s">
         <v>1595</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="8" t="s">
         <v>1596</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="8">
         <v>6.9194535073409504</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="8">
         <v>10</v>
       </c>
-      <c r="F14">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="G14">
+      <c r="F14" s="8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G14" s="8">
         <v>1.1240770196859E-2</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="8">
         <v>1.2020809870938299E-2</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I14" s="8" t="s">
         <v>1597</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J14" s="8" t="s">
         <v>1598</v>
       </c>
       <c r="K14" t="s">
@@ -6663,34 +6739,34 @@
       </c>
     </row>
     <row r="16" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
+      <c r="A16" s="8">
         <v>79</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="8" t="s">
         <v>427</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="8" t="s">
         <v>428</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="8">
         <v>6.1506253398586201</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="8">
         <v>10</v>
       </c>
-      <c r="F16" s="2">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="G16" s="2">
+      <c r="F16" s="8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G16" s="8">
         <v>2.9244110256642498E-3</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16" s="8">
         <v>3.2961093600526502E-3</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="I16" s="8" t="s">
         <v>429</v>
       </c>
-      <c r="J16" s="2" t="s">
+      <c r="J16" s="8" t="s">
         <v>430</v>
       </c>
       <c r="K16" s="2" t="s">
@@ -6778,34 +6854,34 @@
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A18">
+      <c r="A18" s="8">
         <v>226</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="8" t="s">
         <v>1108</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="8" t="s">
         <v>1109</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="8">
         <v>5.6775003137156501</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="8">
         <v>9</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="8">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="8">
         <v>9.8950316650919506E-3</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="8">
         <v>1.0509982930723799E-2</v>
       </c>
-      <c r="I18" t="s">
+      <c r="I18" s="8" t="s">
         <v>1110</v>
       </c>
-      <c r="J18" t="s">
+      <c r="J18" s="8" t="s">
         <v>1111</v>
       </c>
       <c r="K18" t="s">
@@ -6893,33 +6969,34 @@
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A20">
+      <c r="A20" s="8">
         <v>135</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="8" t="s">
         <v>679</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="8" t="s">
         <v>680</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="8">
         <v>5.5355628058727602</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="8">
         <v>10</v>
       </c>
-      <c r="F20">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="G20">
+      <c r="F20" s="8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G20" s="8">
         <v>2.27338256890687E-3</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="8">
         <v>4.7811194271258801E-2</v>
       </c>
-      <c r="I20" t="s">
+      <c r="I20" s="8" t="s">
         <v>681</v>
       </c>
+      <c r="J20" s="8"/>
       <c r="K20" t="s">
         <v>29</v>
       </c>
@@ -6949,34 +7026,34 @@
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A21">
+      <c r="A21" s="8">
         <v>223</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="8" t="s">
         <v>1096</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="8" t="s">
         <v>1097</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="8">
         <v>5.5355628058727602</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="8">
         <v>9</v>
       </c>
-      <c r="F21">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="G21">
+      <c r="F21" s="8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G21" s="8">
         <v>3.6101700667230299E-2</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="8">
         <v>4.1685016467157103E-2</v>
       </c>
-      <c r="I21" t="s">
+      <c r="I21" s="8" t="s">
         <v>1098</v>
       </c>
-      <c r="J21" t="s">
+      <c r="J21" s="8" t="s">
         <v>1099</v>
       </c>
       <c r="K21" t="s">
@@ -7123,34 +7200,34 @@
       </c>
     </row>
     <row r="24" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="3">
+      <c r="A24" s="8">
         <v>311</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="8" t="s">
         <v>1487</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="8" t="s">
         <v>1488</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24" s="8">
         <v>5.2719645770216701</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24" s="8">
         <v>6</v>
       </c>
-      <c r="F24" s="3">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="G24" s="3">
+      <c r="F24" s="8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G24" s="8">
         <v>1.00172765063293E-2</v>
       </c>
-      <c r="H24" s="3">
+      <c r="H24" s="8">
         <v>1.06339454561624E-2</v>
       </c>
-      <c r="I24" s="3" t="s">
+      <c r="I24" s="8" t="s">
         <v>1150</v>
       </c>
-      <c r="J24" s="3" t="s">
+      <c r="J24" s="8" t="s">
         <v>645</v>
       </c>
       <c r="K24" s="3" t="s">
@@ -7182,34 +7259,34 @@
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A25">
+      <c r="A25" s="8">
         <v>268</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="8" t="s">
         <v>1307</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="8" t="s">
         <v>1308</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="8">
         <v>5.1255211165488497</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="8">
         <v>9</v>
       </c>
-      <c r="F25">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="G25">
+      <c r="F25" s="8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G25" s="8">
         <v>2.6097071643107898E-4</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="8">
         <v>1.00397271179678E-2</v>
       </c>
-      <c r="I25" t="s">
+      <c r="I25" s="8" t="s">
         <v>500</v>
       </c>
-      <c r="J25" t="s">
+      <c r="J25" s="8" t="s">
         <v>1309</v>
       </c>
       <c r="K25" t="s">
@@ -7241,33 +7318,34 @@
       </c>
     </row>
     <row r="26" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="4">
+      <c r="A26" s="8">
         <v>66</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="8" t="s">
         <v>363</v>
       </c>
-      <c r="D26" s="4">
+      <c r="D26" s="8">
         <v>5.0323298235206897</v>
       </c>
-      <c r="E26" s="4">
+      <c r="E26" s="8">
         <v>8</v>
       </c>
-      <c r="F26" s="4">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="G26" s="4">
+      <c r="F26" s="8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G26" s="8">
         <v>4.4398257426435201E-3</v>
       </c>
-      <c r="H26" s="4">
+      <c r="H26" s="8">
         <v>4.4398257426435201E-3</v>
       </c>
-      <c r="I26" s="4" t="s">
+      <c r="I26" s="8" t="s">
         <v>364</v>
       </c>
+      <c r="J26" s="8"/>
       <c r="K26" s="4" t="s">
         <v>29</v>
       </c>
@@ -7412,34 +7490,34 @@
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A29">
+      <c r="A29" s="8">
         <v>298</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="8" t="s">
         <v>1435</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="8" t="s">
         <v>1436</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="8">
         <v>4.9678127745011897</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="8">
         <v>6</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="8">
         <v>7.4999999999999997E-3</v>
       </c>
-      <c r="G29">
+      <c r="G29" s="8">
         <v>1.86638759316206E-2</v>
       </c>
-      <c r="H29">
+      <c r="H29" s="8">
         <v>4.7346414278462298E-2</v>
       </c>
-      <c r="I29" t="s">
+      <c r="I29" s="8" t="s">
         <v>1437</v>
       </c>
-      <c r="J29" t="s">
+      <c r="J29" s="8" t="s">
         <v>1438</v>
       </c>
       <c r="K29" t="s">
@@ -7530,34 +7608,34 @@
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A31">
+      <c r="A31" s="8">
         <v>247</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="8" t="s">
         <v>1193</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="8" t="s">
         <v>1194</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="8">
         <v>4.8557568472568002</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="8">
         <v>10</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="8">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="G31">
+      <c r="G31" s="8">
         <v>1.9627531298675501E-3</v>
       </c>
-      <c r="H31">
+      <c r="H31" s="8">
         <v>8.87673532059635E-3</v>
       </c>
-      <c r="I31" t="s">
+      <c r="I31" s="8" t="s">
         <v>1195</v>
       </c>
-      <c r="J31" t="s">
+      <c r="J31" s="8" t="s">
         <v>1196</v>
       </c>
       <c r="K31" t="s">
@@ -7589,34 +7667,34 @@
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A32">
+      <c r="A32" s="8">
         <v>174</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="8" t="s">
         <v>863</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="8" t="s">
         <v>864</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="8">
         <v>4.6129690048939596</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="8">
         <v>10</v>
       </c>
-      <c r="F32">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="G32">
+      <c r="F32" s="8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G32" s="8">
         <v>3.0254766358787901E-2</v>
       </c>
-      <c r="H32">
+      <c r="H32" s="8">
         <v>3.5243098773290397E-2</v>
       </c>
-      <c r="I32" t="s">
+      <c r="I32" s="8" t="s">
         <v>865</v>
       </c>
-      <c r="J32" t="s">
+      <c r="J32" s="8" t="s">
         <v>866</v>
       </c>
       <c r="K32" t="s">
@@ -10120,521 +10198,525 @@
       </c>
     </row>
     <row r="75" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="2">
+      <c r="A75" s="10">
         <v>93</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="B75" s="10" t="s">
         <v>505</v>
       </c>
-      <c r="C75" s="2" t="s">
+      <c r="C75" s="10" t="s">
         <v>506</v>
       </c>
-      <c r="D75" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E75" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F75" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G75" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H75" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="I75" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J75" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="K75" s="2">
+      <c r="D75" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E75" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F75" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G75" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H75" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="I75" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="J75" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="K75" s="10">
         <v>12.182014001077</v>
       </c>
-      <c r="L75" s="2">
+      <c r="L75" s="10">
         <v>10</v>
       </c>
-      <c r="M75" s="2">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="N75" s="2">
+      <c r="M75" s="10">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N75" s="10">
         <v>1.9506265794245301E-4</v>
       </c>
-      <c r="O75" s="2">
+      <c r="O75" s="10">
         <v>3.31183385437561E-2</v>
       </c>
-      <c r="P75" s="2" t="s">
+      <c r="P75" s="10" t="s">
         <v>504</v>
       </c>
-      <c r="R75" s="2">
+      <c r="Q75" s="10"/>
+      <c r="R75" s="10">
         <v>1.9506265794245301E-4</v>
       </c>
-      <c r="S75" s="2" t="s">
+      <c r="S75" s="10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="76" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="2">
+      <c r="A76" s="10">
         <v>94</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="B76" s="10" t="s">
         <v>507</v>
       </c>
-      <c r="C76" s="2" t="s">
+      <c r="C76" s="10" t="s">
         <v>508</v>
       </c>
-      <c r="D76" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E76" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F76" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G76" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H76" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="I76" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J76" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="K76" s="2">
+      <c r="D76" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E76" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F76" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G76" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H76" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="I76" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="J76" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="K76" s="10">
         <v>12.182014001077</v>
       </c>
-      <c r="L76" s="2">
+      <c r="L76" s="10">
         <v>10</v>
       </c>
-      <c r="M76" s="2">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="N76" s="2">
+      <c r="M76" s="10">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N76" s="10">
         <v>1.9506265794245301E-4</v>
       </c>
-      <c r="O76" s="2">
+      <c r="O76" s="10">
         <v>3.31183385437561E-2</v>
       </c>
-      <c r="P76" s="2" t="s">
+      <c r="P76" s="10" t="s">
         <v>504</v>
       </c>
-      <c r="R76" s="2">
+      <c r="Q76" s="10"/>
+      <c r="R76" s="10">
         <v>1.9506265794245301E-4</v>
       </c>
-      <c r="S76" s="2" t="s">
+      <c r="S76" s="10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="77" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="2">
+      <c r="A77" s="10">
         <v>239</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="B77" s="10" t="s">
         <v>1165</v>
       </c>
-      <c r="C77" s="2" t="s">
+      <c r="C77" s="10" t="s">
         <v>1166</v>
       </c>
-      <c r="D77" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E77" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F77" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G77" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H77" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="I77" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J77" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="K77" s="2">
+      <c r="D77" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E77" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F77" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G77" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H77" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="I77" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="J77" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="K77" s="10">
         <v>11.420638126009701</v>
       </c>
-      <c r="L77" s="2">
+      <c r="L77" s="10">
         <v>10</v>
       </c>
-      <c r="M77" s="2">
+      <c r="M77" s="10">
         <v>7.4999999999999997E-3</v>
       </c>
-      <c r="N77" s="2">
+      <c r="N77" s="10">
         <v>1.7934742786836501E-4</v>
       </c>
-      <c r="O77" s="2">
+      <c r="O77" s="10">
         <v>1.08636726407958E-2</v>
       </c>
-      <c r="P77" s="2" t="s">
+      <c r="P77" s="10" t="s">
         <v>1167</v>
       </c>
-      <c r="Q77" s="2" t="s">
+      <c r="Q77" s="10" t="s">
         <v>801</v>
       </c>
-      <c r="R77" s="2">
+      <c r="R77" s="10">
         <v>1.7934742786836501E-4</v>
       </c>
-      <c r="S77" s="2" t="s">
+      <c r="S77" s="10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="78" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A78">
+      <c r="A78" s="10">
         <v>160</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B78" s="10" t="s">
         <v>799</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C78" s="10" t="s">
         <v>800</v>
       </c>
-      <c r="D78" t="s">
-        <v>29</v>
-      </c>
-      <c r="E78" t="s">
-        <v>29</v>
-      </c>
-      <c r="F78" t="s">
-        <v>29</v>
-      </c>
-      <c r="G78" t="s">
-        <v>29</v>
-      </c>
-      <c r="H78" t="s">
-        <v>29</v>
-      </c>
-      <c r="I78" t="s">
-        <v>29</v>
-      </c>
-      <c r="J78" t="s">
-        <v>29</v>
-      </c>
-      <c r="K78">
+      <c r="D78" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E78" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F78" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G78" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H78" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="I78" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="J78" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="K78" s="10">
         <v>10.9638126009693</v>
       </c>
-      <c r="L78">
+      <c r="L78" s="10">
         <v>7</v>
       </c>
-      <c r="M78">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="N78">
+      <c r="M78" s="10">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N78" s="10">
         <v>4.9963117570514396E-3</v>
       </c>
-      <c r="O78">
+      <c r="O78" s="10">
         <v>5.7885275829484498E-3</v>
       </c>
-      <c r="P78" t="s">
+      <c r="P78" s="10" t="s">
         <v>758</v>
       </c>
-      <c r="Q78" t="s">
+      <c r="Q78" s="10" t="s">
         <v>801</v>
       </c>
-      <c r="R78">
+      <c r="R78" s="10">
         <v>4.9963117570514396E-3</v>
       </c>
-      <c r="S78" t="s">
+      <c r="S78" s="10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="79" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="2">
+      <c r="A79" s="10">
         <v>305</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="B79" s="10" t="s">
         <v>1465</v>
       </c>
-      <c r="C79" s="2" t="s">
+      <c r="C79" s="10" t="s">
         <v>1466</v>
       </c>
-      <c r="D79" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E79" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F79" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G79" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H79" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="I79" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J79" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="K79" s="2">
+      <c r="D79" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E79" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F79" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G79" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H79" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="I79" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="J79" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="K79" s="10">
         <v>10.9638126009693</v>
       </c>
-      <c r="L79" s="2">
+      <c r="L79" s="10">
         <v>10</v>
       </c>
-      <c r="M79" s="2">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="N79" s="5" t="s">
+      <c r="M79" s="10">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N79" s="11" t="s">
         <v>1467</v>
       </c>
-      <c r="O79" s="2">
+      <c r="O79" s="10">
         <v>1.6656302882084601E-2</v>
       </c>
-      <c r="P79" s="2" t="s">
+      <c r="P79" s="10" t="s">
         <v>1167</v>
       </c>
-      <c r="R79" s="5" t="s">
+      <c r="Q79" s="10"/>
+      <c r="R79" s="11" t="s">
         <v>1468</v>
       </c>
-      <c r="S79" s="2" t="s">
+      <c r="S79" s="10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="80" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A80">
+      <c r="A80" s="10">
         <v>321</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B80" s="10" t="s">
         <v>1524</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C80" s="10" t="s">
         <v>1525</v>
       </c>
-      <c r="D80" t="s">
-        <v>29</v>
-      </c>
-      <c r="E80" t="s">
-        <v>29</v>
-      </c>
-      <c r="F80" t="s">
-        <v>29</v>
-      </c>
-      <c r="G80" t="s">
-        <v>29</v>
-      </c>
-      <c r="H80" t="s">
-        <v>29</v>
-      </c>
-      <c r="I80" t="s">
-        <v>29</v>
-      </c>
-      <c r="J80" t="s">
-        <v>29</v>
-      </c>
-      <c r="K80">
+      <c r="D80" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E80" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F80" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G80" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H80" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="I80" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="J80" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="K80" s="10">
         <v>10.9638126009693</v>
       </c>
-      <c r="L80">
+      <c r="L80" s="10">
         <v>8</v>
       </c>
-      <c r="M80">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="N80">
+      <c r="M80" s="10">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N80" s="10">
         <v>1.76127338351206E-3</v>
       </c>
-      <c r="O80">
+      <c r="O80" s="10">
         <v>3.0100396027309101E-2</v>
       </c>
-      <c r="P80" t="s">
+      <c r="P80" s="10" t="s">
         <v>1526</v>
       </c>
-      <c r="Q80" t="s">
+      <c r="Q80" s="10" t="s">
         <v>1527</v>
       </c>
-      <c r="R80">
+      <c r="R80" s="10">
         <v>1.76127338351206E-3</v>
       </c>
-      <c r="S80" t="s">
+      <c r="S80" s="10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="81" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A81">
+      <c r="A81" s="10">
         <v>286</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B81" s="10" t="s">
         <v>1384</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C81" s="10" t="s">
         <v>1385</v>
       </c>
-      <c r="D81" t="s">
-        <v>29</v>
-      </c>
-      <c r="E81" t="s">
-        <v>29</v>
-      </c>
-      <c r="F81" t="s">
-        <v>29</v>
-      </c>
-      <c r="G81" t="s">
-        <v>29</v>
-      </c>
-      <c r="H81" t="s">
-        <v>29</v>
-      </c>
-      <c r="I81" t="s">
-        <v>29</v>
-      </c>
-      <c r="J81" t="s">
-        <v>29</v>
-      </c>
-      <c r="K81">
+      <c r="D81" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E81" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F81" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G81" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H81" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="I81" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="J81" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="K81" s="10">
         <v>10.659262250942399</v>
       </c>
-      <c r="L81">
+      <c r="L81" s="10">
         <v>10</v>
       </c>
-      <c r="M81">
+      <c r="M81" s="10">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="N81" s="1" t="s">
+      <c r="N81" s="11" t="s">
         <v>1386</v>
       </c>
-      <c r="O81" s="1" t="s">
+      <c r="O81" s="11" t="s">
         <v>1031</v>
       </c>
-      <c r="P81" t="s">
+      <c r="P81" s="10" t="s">
         <v>1387</v>
       </c>
-      <c r="Q81" t="s">
+      <c r="Q81" s="10" t="s">
         <v>1388</v>
       </c>
-      <c r="R81" s="1" t="s">
+      <c r="R81" s="11" t="s">
         <v>1386</v>
       </c>
-      <c r="S81" t="s">
+      <c r="S81" s="10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="82" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A82">
+      <c r="A82" s="10">
         <v>92</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B82" s="10" t="s">
         <v>502</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C82" s="10" t="s">
         <v>503</v>
       </c>
-      <c r="D82" t="s">
-        <v>29</v>
-      </c>
-      <c r="E82" t="s">
-        <v>29</v>
-      </c>
-      <c r="F82" t="s">
-        <v>29</v>
-      </c>
-      <c r="G82" t="s">
-        <v>29</v>
-      </c>
-      <c r="H82" t="s">
-        <v>29</v>
-      </c>
-      <c r="I82" t="s">
-        <v>29</v>
-      </c>
-      <c r="J82" t="s">
-        <v>29</v>
-      </c>
-      <c r="K82">
+      <c r="D82" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E82" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F82" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G82" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H82" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="I82" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="J82" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="K82" s="10">
         <v>10.441726286637399</v>
       </c>
-      <c r="L82">
+      <c r="L82" s="10">
         <v>8</v>
       </c>
-      <c r="M82">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="N82">
+      <c r="M82" s="10">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N82" s="10">
         <v>3.4102011929054699E-4</v>
       </c>
-      <c r="O82">
+      <c r="O82" s="10">
         <v>2.64138216602594E-2</v>
       </c>
-      <c r="P82" t="s">
+      <c r="P82" s="10" t="s">
         <v>504</v>
       </c>
-      <c r="R82">
+      <c r="Q82" s="10"/>
+      <c r="R82" s="10">
         <v>3.4102011929054802E-4</v>
       </c>
-      <c r="S82" t="s">
+      <c r="S82" s="10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="83" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A83">
+      <c r="A83" s="10">
         <v>76</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B83" s="10" t="s">
         <v>415</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C83" s="10" t="s">
         <v>416</v>
       </c>
-      <c r="D83" t="s">
-        <v>29</v>
-      </c>
-      <c r="E83" t="s">
-        <v>29</v>
-      </c>
-      <c r="F83" t="s">
-        <v>29</v>
-      </c>
-      <c r="G83" t="s">
-        <v>29</v>
-      </c>
-      <c r="H83" t="s">
-        <v>29</v>
-      </c>
-      <c r="I83" t="s">
-        <v>29</v>
-      </c>
-      <c r="J83" t="s">
-        <v>29</v>
-      </c>
-      <c r="K83">
+      <c r="D83" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E83" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F83" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G83" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H83" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="I83" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="J83" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="K83" s="10">
         <v>9.1365105008077592</v>
       </c>
-      <c r="L83">
+      <c r="L83" s="10">
         <v>9</v>
       </c>
-      <c r="M83">
+      <c r="M83" s="10">
         <v>0.01</v>
       </c>
-      <c r="N83">
+      <c r="N83" s="10">
         <v>6.2343823399003105E-4</v>
       </c>
-      <c r="O83">
+      <c r="O83" s="10">
         <v>3.8017056899195198E-2</v>
       </c>
-      <c r="P83" t="s">
+      <c r="P83" s="10" t="s">
         <v>417</v>
       </c>
-      <c r="Q83" t="s">
+      <c r="Q83" s="10" t="s">
         <v>418</v>
       </c>
-      <c r="R83">
+      <c r="R83" s="10">
         <v>6.2343823399003105E-4</v>
       </c>
-      <c r="S83" t="s">
+      <c r="S83" s="10" t="s">
         <v>32</v>
       </c>
     </row>
@@ -10695,117 +10777,118 @@
       </c>
     </row>
     <row r="85" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A85">
+      <c r="A85" s="10">
         <v>184</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B85" s="10" t="s">
         <v>906</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C85" s="10" t="s">
         <v>907</v>
       </c>
-      <c r="D85" t="s">
-        <v>29</v>
-      </c>
-      <c r="E85" t="s">
-        <v>29</v>
-      </c>
-      <c r="F85" t="s">
-        <v>29</v>
-      </c>
-      <c r="G85" t="s">
-        <v>29</v>
-      </c>
-      <c r="H85" t="s">
-        <v>29</v>
-      </c>
-      <c r="I85" t="s">
-        <v>29</v>
-      </c>
-      <c r="J85" t="s">
-        <v>29</v>
-      </c>
-      <c r="K85">
+      <c r="D85" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E85" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F85" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G85" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H85" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="I85" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="J85" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="K85" s="10">
         <v>9.1365105008077592</v>
       </c>
-      <c r="L85">
+      <c r="L85" s="10">
         <v>10</v>
       </c>
-      <c r="M85">
+      <c r="M85" s="10">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="N85">
+      <c r="N85" s="10">
         <v>1.41550969110565E-3</v>
       </c>
-      <c r="O85">
+      <c r="O85" s="10">
         <v>2.5938533693604202E-2</v>
       </c>
-      <c r="P85" t="s">
+      <c r="P85" s="10" t="s">
         <v>908</v>
       </c>
-      <c r="R85">
+      <c r="Q85" s="10"/>
+      <c r="R85" s="10">
         <v>1.41550969110565E-3</v>
       </c>
-      <c r="S85" t="s">
+      <c r="S85" s="10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="86" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A86">
+      <c r="A86" s="10">
         <v>203</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B86" s="10" t="s">
         <v>1008</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C86" s="10" t="s">
         <v>1009</v>
       </c>
-      <c r="D86" t="s">
-        <v>29</v>
-      </c>
-      <c r="E86" t="s">
-        <v>29</v>
-      </c>
-      <c r="F86" t="s">
-        <v>29</v>
-      </c>
-      <c r="G86" t="s">
-        <v>29</v>
-      </c>
-      <c r="H86" t="s">
-        <v>29</v>
-      </c>
-      <c r="I86" t="s">
-        <v>29</v>
-      </c>
-      <c r="J86" t="s">
-        <v>29</v>
-      </c>
-      <c r="K86">
+      <c r="D86" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E86" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F86" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G86" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H86" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="I86" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="J86" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="K86" s="10">
         <v>9.1365105008077592</v>
       </c>
-      <c r="L86">
+      <c r="L86" s="10">
         <v>10</v>
       </c>
-      <c r="M86">
+      <c r="M86" s="10">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="N86">
+      <c r="N86" s="10">
         <v>3.05878163512454E-4</v>
       </c>
-      <c r="O86">
+      <c r="O86" s="10">
         <v>4.5467445971468998E-3</v>
       </c>
-      <c r="P86" t="s">
+      <c r="P86" s="10" t="s">
         <v>1010</v>
       </c>
-      <c r="Q86" t="s">
+      <c r="Q86" s="10" t="s">
         <v>1011</v>
       </c>
-      <c r="R86">
+      <c r="R86" s="10">
         <v>3.05878163512454E-4</v>
       </c>
-      <c r="S86" t="s">
+      <c r="S86" s="10" t="s">
         <v>32</v>
       </c>
     </row>
@@ -10984,61 +11067,61 @@
       </c>
     </row>
     <row r="90" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A90">
+      <c r="A90" s="10">
         <v>270</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B90" s="10" t="s">
         <v>1312</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C90" s="10" t="s">
         <v>1313</v>
       </c>
-      <c r="D90" t="s">
-        <v>29</v>
-      </c>
-      <c r="E90" t="s">
-        <v>29</v>
-      </c>
-      <c r="F90" t="s">
-        <v>29</v>
-      </c>
-      <c r="G90" t="s">
-        <v>29</v>
-      </c>
-      <c r="H90" t="s">
-        <v>29</v>
-      </c>
-      <c r="I90" t="s">
-        <v>29</v>
-      </c>
-      <c r="J90" t="s">
-        <v>29</v>
-      </c>
-      <c r="K90">
+      <c r="D90" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E90" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F90" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G90" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H90" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="I90" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="J90" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="K90" s="10">
         <v>8.1213426673846705</v>
       </c>
-      <c r="L90">
+      <c r="L90" s="10">
         <v>10</v>
       </c>
-      <c r="M90">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="N90" s="1" t="s">
+      <c r="M90" s="10">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N90" s="11" t="s">
         <v>1314</v>
       </c>
-      <c r="O90">
+      <c r="O90" s="10">
         <v>1.6017496821703E-3</v>
       </c>
-      <c r="P90" t="s">
+      <c r="P90" s="10" t="s">
         <v>1167</v>
       </c>
-      <c r="Q90" t="s">
+      <c r="Q90" s="10" t="s">
         <v>634</v>
       </c>
-      <c r="R90" s="1" t="s">
+      <c r="R90" s="11" t="s">
         <v>1314</v>
       </c>
-      <c r="S90" t="s">
+      <c r="S90" s="10" t="s">
         <v>32</v>
       </c>
     </row>
@@ -11158,415 +11241,415 @@
       </c>
     </row>
     <row r="93" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A93">
+      <c r="A93" s="10">
         <v>148</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B93" s="10" t="s">
         <v>743</v>
       </c>
-      <c r="C93" t="s">
+      <c r="C93" s="10" t="s">
         <v>744</v>
       </c>
-      <c r="D93" t="s">
-        <v>29</v>
-      </c>
-      <c r="E93" t="s">
-        <v>29</v>
-      </c>
-      <c r="F93" t="s">
-        <v>29</v>
-      </c>
-      <c r="G93" t="s">
-        <v>29</v>
-      </c>
-      <c r="H93" t="s">
-        <v>29</v>
-      </c>
-      <c r="I93" t="s">
-        <v>29</v>
-      </c>
-      <c r="J93" t="s">
-        <v>29</v>
-      </c>
-      <c r="K93">
+      <c r="D93" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E93" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F93" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G93" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H93" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="I93" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="J93" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="K93" s="10">
         <v>7.8312947149780703</v>
       </c>
-      <c r="L93">
+      <c r="L93" s="10">
         <v>10</v>
       </c>
-      <c r="M93">
+      <c r="M93" s="10">
         <v>0.01</v>
       </c>
-      <c r="N93">
+      <c r="N93" s="10">
         <v>2.4722151837369799E-3</v>
       </c>
-      <c r="O93">
+      <c r="O93" s="10">
         <v>3.1930852281499597E-2</v>
       </c>
-      <c r="P93" t="s">
+      <c r="P93" s="10" t="s">
         <v>745</v>
       </c>
-      <c r="Q93" t="s">
+      <c r="Q93" s="10" t="s">
         <v>746</v>
       </c>
-      <c r="R93">
+      <c r="R93" s="10">
         <v>2.4722151837369799E-3</v>
       </c>
-      <c r="S93" t="s">
+      <c r="S93" s="10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="94" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A94">
+      <c r="A94" s="10">
         <v>153</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B94" s="10" t="s">
         <v>763</v>
       </c>
-      <c r="C94" t="s">
+      <c r="C94" s="10" t="s">
         <v>764</v>
       </c>
-      <c r="D94" t="s">
-        <v>29</v>
-      </c>
-      <c r="E94" t="s">
-        <v>29</v>
-      </c>
-      <c r="F94" t="s">
-        <v>29</v>
-      </c>
-      <c r="G94" t="s">
-        <v>29</v>
-      </c>
-      <c r="H94" t="s">
-        <v>29</v>
-      </c>
-      <c r="I94" t="s">
-        <v>29</v>
-      </c>
-      <c r="J94" t="s">
-        <v>29</v>
-      </c>
-      <c r="K94">
+      <c r="D94" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E94" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F94" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G94" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H94" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="I94" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="J94" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="K94" s="10">
         <v>7.8312947149780703</v>
       </c>
-      <c r="L94">
+      <c r="L94" s="10">
         <v>10</v>
       </c>
-      <c r="M94">
+      <c r="M94" s="10">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="N94">
+      <c r="N94" s="10">
         <v>2.2411590660983498E-3</v>
       </c>
-      <c r="O94">
+      <c r="O94" s="10">
         <v>1.7351748497455799E-2</v>
       </c>
-      <c r="P94" t="s">
+      <c r="P94" s="10" t="s">
         <v>765</v>
       </c>
-      <c r="Q94" t="s">
+      <c r="Q94" s="10" t="s">
         <v>766</v>
       </c>
-      <c r="R94">
+      <c r="R94" s="10">
         <v>2.2411590660983498E-3</v>
       </c>
-      <c r="S94" t="s">
+      <c r="S94" s="10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="95" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A95">
+      <c r="A95" s="10">
         <v>168</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B95" s="10" t="s">
         <v>835</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C95" s="10" t="s">
         <v>836</v>
       </c>
-      <c r="D95" t="s">
-        <v>29</v>
-      </c>
-      <c r="E95" t="s">
-        <v>29</v>
-      </c>
-      <c r="F95" t="s">
-        <v>29</v>
-      </c>
-      <c r="G95" t="s">
-        <v>29</v>
-      </c>
-      <c r="H95" t="s">
-        <v>29</v>
-      </c>
-      <c r="I95" t="s">
-        <v>29</v>
-      </c>
-      <c r="J95" t="s">
-        <v>29</v>
-      </c>
-      <c r="K95">
+      <c r="D95" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E95" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F95" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G95" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H95" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="I95" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="J95" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="K95" s="10">
         <v>7.8312947149780703</v>
       </c>
-      <c r="L95">
+      <c r="L95" s="10">
         <v>10</v>
       </c>
-      <c r="M95">
+      <c r="M95" s="10">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="N95" s="1" t="s">
+      <c r="N95" s="11" t="s">
         <v>837</v>
       </c>
-      <c r="O95">
+      <c r="O95" s="10">
         <v>1.9742113317538601E-4</v>
       </c>
-      <c r="P95" t="s">
+      <c r="P95" s="10" t="s">
         <v>838</v>
       </c>
-      <c r="Q95" t="s">
+      <c r="Q95" s="10" t="s">
         <v>839</v>
       </c>
-      <c r="R95" s="1" t="s">
+      <c r="R95" s="11" t="s">
         <v>837</v>
       </c>
-      <c r="S95" t="s">
+      <c r="S95" s="10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="96" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A96">
+      <c r="A96" s="10">
         <v>259</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B96" s="10" t="s">
         <v>1257</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C96" s="10" t="s">
         <v>1258</v>
       </c>
-      <c r="D96" t="s">
-        <v>29</v>
-      </c>
-      <c r="E96" t="s">
-        <v>29</v>
-      </c>
-      <c r="F96" t="s">
-        <v>29</v>
-      </c>
-      <c r="G96" t="s">
-        <v>29</v>
-      </c>
-      <c r="H96" t="s">
-        <v>29</v>
-      </c>
-      <c r="I96" t="s">
-        <v>29</v>
-      </c>
-      <c r="J96" t="s">
-        <v>29</v>
-      </c>
-      <c r="K96">
+      <c r="D96" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E96" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F96" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G96" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H96" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="I96" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="J96" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="K96" s="10">
         <v>7.3092084006461997</v>
       </c>
-      <c r="L96">
+      <c r="L96" s="10">
         <v>10</v>
       </c>
-      <c r="M96">
+      <c r="M96" s="10">
         <v>0.01</v>
       </c>
-      <c r="N96">
+      <c r="N96" s="10">
         <v>5.7711772687302799E-3</v>
       </c>
-      <c r="O96">
+      <c r="O96" s="10">
         <v>3.9839748188947303E-2</v>
       </c>
-      <c r="P96" t="s">
+      <c r="P96" s="10" t="s">
         <v>1259</v>
       </c>
-      <c r="Q96" t="s">
+      <c r="Q96" s="10" t="s">
         <v>1260</v>
       </c>
-      <c r="R96">
+      <c r="R96" s="10">
         <v>5.7711772687302799E-3</v>
       </c>
-      <c r="S96" t="s">
+      <c r="S96" s="10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="97" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A97">
+      <c r="A97" s="10">
         <v>257</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B97" s="10" t="s">
         <v>1246</v>
       </c>
-      <c r="C97" t="s">
+      <c r="C97" s="10" t="s">
         <v>1247</v>
       </c>
-      <c r="D97" t="s">
-        <v>29</v>
-      </c>
-      <c r="E97" t="s">
-        <v>29</v>
-      </c>
-      <c r="F97" t="s">
-        <v>29</v>
-      </c>
-      <c r="G97" t="s">
-        <v>29</v>
-      </c>
-      <c r="H97" t="s">
-        <v>29</v>
-      </c>
-      <c r="I97" t="s">
-        <v>29</v>
-      </c>
-      <c r="J97" t="s">
-        <v>29</v>
-      </c>
-      <c r="K97">
+      <c r="D97" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E97" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F97" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G97" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H97" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="I97" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="J97" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="K97" s="10">
         <v>6.9611508577582901</v>
       </c>
-      <c r="L97">
+      <c r="L97" s="10">
         <v>10</v>
       </c>
-      <c r="M97">
+      <c r="M97" s="10">
         <v>0.04</v>
       </c>
-      <c r="N97" s="1" t="s">
+      <c r="N97" s="11" t="s">
         <v>1248</v>
       </c>
-      <c r="O97">
+      <c r="O97" s="10">
         <v>2.0226110130846099E-3</v>
       </c>
-      <c r="P97" t="s">
+      <c r="P97" s="10" t="s">
         <v>1249</v>
       </c>
-      <c r="Q97" t="s">
+      <c r="Q97" s="10" t="s">
         <v>1250</v>
       </c>
-      <c r="R97" s="1" t="s">
+      <c r="R97" s="11" t="s">
         <v>1248</v>
       </c>
-      <c r="S97" t="s">
+      <c r="S97" s="10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="98" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A98">
+      <c r="A98" s="10">
         <v>17</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B98" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C98" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="D98" t="s">
-        <v>29</v>
-      </c>
-      <c r="E98" t="s">
-        <v>29</v>
-      </c>
-      <c r="F98" t="s">
-        <v>29</v>
-      </c>
-      <c r="G98" t="s">
-        <v>29</v>
-      </c>
-      <c r="H98" t="s">
-        <v>29</v>
-      </c>
-      <c r="I98" t="s">
-        <v>29</v>
-      </c>
-      <c r="J98" t="s">
-        <v>29</v>
-      </c>
-      <c r="K98">
+      <c r="D98" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E98" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F98" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G98" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H98" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="I98" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="J98" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="K98" s="10">
         <v>6.8523828756058203</v>
       </c>
-      <c r="L98">
+      <c r="L98" s="10">
         <v>8</v>
       </c>
-      <c r="M98">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="N98">
+      <c r="M98" s="10">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N98" s="10">
         <v>1.39917330503368E-2</v>
       </c>
-      <c r="O98">
+      <c r="O98" s="10">
         <v>3.8853346683334102E-2</v>
       </c>
-      <c r="P98" t="s">
+      <c r="P98" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="Q98" t="s">
+      <c r="Q98" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="R98">
+      <c r="R98" s="10">
         <v>1.39917330503368E-2</v>
       </c>
-      <c r="S98" t="s">
+      <c r="S98" s="10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="99" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A99">
+      <c r="A99" s="10">
         <v>101</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B99" s="10" t="s">
         <v>533</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C99" s="10" t="s">
         <v>534</v>
       </c>
-      <c r="D99" t="s">
-        <v>29</v>
-      </c>
-      <c r="E99" t="s">
-        <v>29</v>
-      </c>
-      <c r="F99" t="s">
-        <v>29</v>
-      </c>
-      <c r="G99" t="s">
-        <v>29</v>
-      </c>
-      <c r="H99" t="s">
-        <v>29</v>
-      </c>
-      <c r="I99" t="s">
-        <v>29</v>
-      </c>
-      <c r="J99" t="s">
-        <v>29</v>
-      </c>
-      <c r="K99">
+      <c r="D99" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E99" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F99" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G99" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H99" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="I99" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="J99" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="K99" s="10">
         <v>6.8523828756058203</v>
       </c>
-      <c r="L99">
+      <c r="L99" s="10">
         <v>9</v>
       </c>
-      <c r="M99">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="N99">
+      <c r="M99" s="10">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N99" s="10">
         <v>9.7829325086427402E-3</v>
       </c>
-      <c r="O99">
+      <c r="O99" s="10">
         <v>3.9388845697973997E-2</v>
       </c>
-      <c r="P99" t="s">
+      <c r="P99" s="10" t="s">
         <v>535</v>
       </c>
-      <c r="Q99" t="s">
+      <c r="Q99" s="10" t="s">
         <v>536</v>
       </c>
-      <c r="R99">
+      <c r="R99" s="10">
         <v>9.7829325086427402E-3</v>
       </c>
-      <c r="S99" t="s">
+      <c r="S99" s="10" t="s">
         <v>32</v>
       </c>
     </row>
@@ -11630,61 +11713,61 @@
       </c>
     </row>
     <row r="101" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A101">
+      <c r="A101" s="10">
         <v>217</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B101" s="10" t="s">
         <v>1066</v>
       </c>
-      <c r="C101" t="s">
+      <c r="C101" s="10" t="s">
         <v>1067</v>
       </c>
-      <c r="D101" t="s">
-        <v>29</v>
-      </c>
-      <c r="E101" t="s">
-        <v>29</v>
-      </c>
-      <c r="F101" t="s">
-        <v>29</v>
-      </c>
-      <c r="G101" t="s">
-        <v>29</v>
-      </c>
-      <c r="H101" t="s">
-        <v>29</v>
-      </c>
-      <c r="I101" t="s">
-        <v>29</v>
-      </c>
-      <c r="J101" t="s">
-        <v>29</v>
-      </c>
-      <c r="K101">
+      <c r="D101" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E101" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F101" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G101" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H101" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="I101" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="J101" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="K101" s="10">
         <v>6.5260789291484</v>
       </c>
-      <c r="L101">
+      <c r="L101" s="10">
         <v>10</v>
       </c>
-      <c r="M101">
+      <c r="M101" s="10">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="N101">
+      <c r="N101" s="10">
         <v>5.6714615027162005E-4</v>
       </c>
-      <c r="O101">
+      <c r="O101" s="10">
         <v>2.53553493609644E-2</v>
       </c>
-      <c r="P101" t="s">
+      <c r="P101" s="10" t="s">
         <v>1068</v>
       </c>
-      <c r="Q101" t="s">
+      <c r="Q101" s="10" t="s">
         <v>1069</v>
       </c>
-      <c r="R101">
+      <c r="R101" s="10">
         <v>5.6714615027162005E-4</v>
       </c>
-      <c r="S101" t="s">
+      <c r="S101" s="10" t="s">
         <v>32</v>
       </c>
     </row>
@@ -17879,56 +17962,56 @@
         <v>32</v>
       </c>
     </row>
-    <row r="208" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A208">
+    <row r="208" spans="1:19" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A208" s="17">
         <v>127</v>
       </c>
-      <c r="B208" t="s">
+      <c r="B208" s="17" t="s">
         <v>646</v>
       </c>
-      <c r="C208" t="s">
+      <c r="C208" s="17" t="s">
         <v>647</v>
       </c>
-      <c r="D208">
+      <c r="D208" s="17">
         <v>13.838907014681901</v>
       </c>
-      <c r="E208">
+      <c r="E208" s="17">
         <v>10</v>
       </c>
-      <c r="F208">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="G208">
+      <c r="F208" s="17">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G208" s="17">
         <v>1.6958502116737599E-2</v>
       </c>
-      <c r="H208">
+      <c r="H208" s="17">
         <v>3.3571666837698799E-2</v>
       </c>
-      <c r="I208" t="s">
+      <c r="I208" s="17" t="s">
         <v>648</v>
       </c>
-      <c r="K208">
+      <c r="K208" s="17">
         <v>11.420638126009701</v>
       </c>
-      <c r="L208">
+      <c r="L208" s="17">
         <v>6</v>
       </c>
-      <c r="M208">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="N208">
+      <c r="M208" s="17">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N208" s="17">
         <v>3.5333950356294599E-4</v>
       </c>
-      <c r="O208">
+      <c r="O208" s="17">
         <v>4.5836645842928798E-2</v>
       </c>
-      <c r="P208" t="s">
+      <c r="P208" s="17" t="s">
         <v>649</v>
       </c>
-      <c r="R208" s="1" t="s">
+      <c r="R208" s="18" t="s">
         <v>650</v>
       </c>
-      <c r="S208" t="s">
+      <c r="S208" s="17" t="s">
         <v>26</v>
       </c>
     </row>
@@ -19299,7 +19382,7 @@
       <c r="Q232" s="3" t="s">
         <v>1463</v>
       </c>
-      <c r="R232" s="6" t="s">
+      <c r="R232" s="5" t="s">
         <v>1464</v>
       </c>
       <c r="S232" s="3" t="s">
@@ -20070,56 +20153,56 @@
         <v>26</v>
       </c>
     </row>
-    <row r="246" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A246" s="7">
+    <row r="246" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A246" s="6">
         <v>146</v>
       </c>
-      <c r="B246" s="7" t="s">
+      <c r="B246" s="6" t="s">
         <v>733</v>
       </c>
-      <c r="C246" s="7" t="s">
+      <c r="C246" s="6" t="s">
         <v>734</v>
       </c>
-      <c r="D246" s="7">
+      <c r="D246" s="6">
         <v>7.3807504078303401</v>
       </c>
-      <c r="E246" s="7">
+      <c r="E246" s="6">
         <v>10</v>
       </c>
-      <c r="F246" s="7">
+      <c r="F246" s="6">
         <v>0.01</v>
       </c>
-      <c r="G246" s="8" t="s">
+      <c r="G246" s="7" t="s">
         <v>735</v>
       </c>
-      <c r="H246" s="7">
+      <c r="H246" s="6">
         <v>3.4014916077402597E-2</v>
       </c>
-      <c r="I246" s="7" t="s">
+      <c r="I246" s="6" t="s">
         <v>736</v>
       </c>
-      <c r="K246" s="7">
+      <c r="K246" s="6">
         <v>5.48190630048465</v>
       </c>
-      <c r="L246" s="7">
+      <c r="L246" s="6">
         <v>1</v>
       </c>
-      <c r="M246" s="7">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="N246" s="7">
+      <c r="M246" s="6">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N246" s="6">
         <v>4.17122204949713E-3</v>
       </c>
-      <c r="O246" s="7">
+      <c r="O246" s="6">
         <v>4.17122204949713E-3</v>
       </c>
-      <c r="P246" s="7" t="s">
+      <c r="P246" s="6" t="s">
         <v>737</v>
       </c>
-      <c r="R246" s="8" t="s">
+      <c r="R246" s="7" t="s">
         <v>738</v>
       </c>
-      <c r="S246" s="7" t="s">
+      <c r="S246" s="6" t="s">
         <v>26</v>
       </c>
     </row>
@@ -25734,9 +25817,1489 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S344">
-    <sortCondition ref="S1:S344"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S341">
+    <sortCondition ref="S47:S342"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29B590FF-EDF1-2E4E-A9CE-3568C58E3596}">
+  <dimension ref="A1:J21"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" zoomScale="200" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="62.6640625" style="13" customWidth="1"/>
+    <col min="10" max="10" width="26.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="9"/>
+      <c r="B1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="9">
+        <v>38</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="D2" s="9">
+        <v>11.0711256</v>
+      </c>
+      <c r="E2" s="9">
+        <v>9</v>
+      </c>
+      <c r="F2" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="G2" s="9">
+        <v>1.69922E-3</v>
+      </c>
+      <c r="H2" s="9">
+        <v>2.2210980000000002E-2</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="J2" s="9"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="9">
+        <v>338</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>1603</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>1604</v>
+      </c>
+      <c r="D3" s="9">
+        <v>10.543929199999999</v>
+      </c>
+      <c r="E3" s="9">
+        <v>10</v>
+      </c>
+      <c r="F3" s="9">
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="G3" s="9">
+        <v>7.0301000000000001E-4</v>
+      </c>
+      <c r="H3" s="9">
+        <v>3.6002890000000003E-2</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>1605</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>1606</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="9">
+        <v>39</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="D4" s="9">
+        <v>9.2259380100000001</v>
+      </c>
+      <c r="E4" s="9">
+        <v>7</v>
+      </c>
+      <c r="F4" s="9">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G4" s="9">
+        <v>3.3893199999999999E-3</v>
+      </c>
+      <c r="H4" s="9">
+        <v>4.4136450000000001E-2</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="J4" s="9"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="9">
+        <v>227</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>1112</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>1113</v>
+      </c>
+      <c r="D5" s="9">
+        <v>9.2259380100000001</v>
+      </c>
+      <c r="E5" s="9">
+        <v>10</v>
+      </c>
+      <c r="F5" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="G5" s="9">
+        <v>8.8380300000000002E-3</v>
+      </c>
+      <c r="H5" s="9">
+        <v>1.015482E-2</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>1114</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="9">
+        <v>162</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>810</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>811</v>
+      </c>
+      <c r="D6" s="9">
+        <v>8.2008337900000008</v>
+      </c>
+      <c r="E6" s="9">
+        <v>10</v>
+      </c>
+      <c r="F6" s="9">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G6" s="9">
+        <v>2.5354330000000001E-2</v>
+      </c>
+      <c r="H6" s="9">
+        <v>3.358908E-2</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>812</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="9">
+        <v>89</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>487</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>488</v>
+      </c>
+      <c r="D7" s="9">
+        <v>7.90794687</v>
+      </c>
+      <c r="E7" s="9">
+        <v>10</v>
+      </c>
+      <c r="F7" s="9">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G7" s="9">
+        <v>5.9153900000000004E-3</v>
+      </c>
+      <c r="H7" s="9">
+        <v>6.3517499999999998E-3</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>489</v>
+      </c>
+      <c r="J7" s="9"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="9">
+        <v>95</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>509</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>510</v>
+      </c>
+      <c r="D8" s="9">
+        <v>7.90794687</v>
+      </c>
+      <c r="E8" s="9">
+        <v>9</v>
+      </c>
+      <c r="F8" s="9">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G8" s="9">
+        <v>1.063395E-2</v>
+      </c>
+      <c r="H8" s="9">
+        <v>4.5148840000000003E-2</v>
+      </c>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="9">
+        <v>75</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>412</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>413</v>
+      </c>
+      <c r="D9" s="9">
+        <v>6.9194535100000003</v>
+      </c>
+      <c r="E9" s="9">
+        <v>10</v>
+      </c>
+      <c r="F9" s="9">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="G9" s="9">
+        <v>5.9774000000000003E-4</v>
+      </c>
+      <c r="H9" s="9">
+        <v>2.07435E-3</v>
+      </c>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="9">
+        <v>124</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>635</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>636</v>
+      </c>
+      <c r="D10" s="9">
+        <v>6.9194535100000003</v>
+      </c>
+      <c r="E10" s="9">
+        <v>10</v>
+      </c>
+      <c r="F10" s="9">
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="G10" s="9">
+        <v>1.549942E-2</v>
+      </c>
+      <c r="H10" s="9">
+        <v>1.746435E-2</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>637</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="9">
+        <v>336</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>1595</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>1596</v>
+      </c>
+      <c r="D11" s="9">
+        <v>6.9194535100000003</v>
+      </c>
+      <c r="E11" s="9">
+        <v>10</v>
+      </c>
+      <c r="F11" s="9">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G11" s="9">
+        <v>1.1240770000000001E-2</v>
+      </c>
+      <c r="H11" s="9">
+        <v>1.202081E-2</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>1597</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>1598</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="9">
+        <v>79</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>427</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>428</v>
+      </c>
+      <c r="D12" s="9">
+        <v>6.1506253400000004</v>
+      </c>
+      <c r="E12" s="9">
+        <v>10</v>
+      </c>
+      <c r="F12" s="9">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G12" s="9">
+        <v>2.9244100000000001E-3</v>
+      </c>
+      <c r="H12" s="9">
+        <v>3.2961100000000001E-3</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>429</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="9">
+        <v>226</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>1108</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>1109</v>
+      </c>
+      <c r="D13" s="9">
+        <v>5.6775003100000001</v>
+      </c>
+      <c r="E13" s="9">
+        <v>9</v>
+      </c>
+      <c r="F13" s="9">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="G13" s="9">
+        <v>9.8950300000000008E-3</v>
+      </c>
+      <c r="H13" s="9">
+        <v>1.050998E-2</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>1110</v>
+      </c>
+      <c r="J13" s="9" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="9">
+        <v>135</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>679</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>680</v>
+      </c>
+      <c r="D14" s="9">
+        <v>5.5355628100000001</v>
+      </c>
+      <c r="E14" s="9">
+        <v>10</v>
+      </c>
+      <c r="F14" s="9">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G14" s="9">
+        <v>2.2733800000000002E-3</v>
+      </c>
+      <c r="H14" s="9">
+        <v>4.7811190000000003E-2</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>681</v>
+      </c>
+      <c r="J14" s="9"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="9">
+        <v>223</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>1096</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>1097</v>
+      </c>
+      <c r="D15" s="9">
+        <v>5.5355628100000001</v>
+      </c>
+      <c r="E15" s="9">
+        <v>9</v>
+      </c>
+      <c r="F15" s="9">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G15" s="9">
+        <v>3.61017E-2</v>
+      </c>
+      <c r="H15" s="9">
+        <v>4.1685020000000003E-2</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>1098</v>
+      </c>
+      <c r="J15" s="9" t="s">
+        <v>1099</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="9">
+        <v>311</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>1487</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>1488</v>
+      </c>
+      <c r="D16" s="9">
+        <v>5.2719645799999997</v>
+      </c>
+      <c r="E16" s="9">
+        <v>6</v>
+      </c>
+      <c r="F16" s="9">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G16" s="9">
+        <v>1.001728E-2</v>
+      </c>
+      <c r="H16" s="9">
+        <v>1.063395E-2</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>1150</v>
+      </c>
+      <c r="J16" s="9" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="9">
+        <v>268</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>1307</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>1308</v>
+      </c>
+      <c r="D17" s="9">
+        <v>5.1255211200000002</v>
+      </c>
+      <c r="E17" s="9">
+        <v>9</v>
+      </c>
+      <c r="F17" s="9">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G17" s="9">
+        <v>2.6097000000000002E-4</v>
+      </c>
+      <c r="H17" s="9">
+        <v>1.003973E-2</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>500</v>
+      </c>
+      <c r="J17" s="9" t="s">
+        <v>1309</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="9">
+        <v>66</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>362</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>363</v>
+      </c>
+      <c r="D18" s="9">
+        <v>5.0323298200000002</v>
+      </c>
+      <c r="E18" s="9">
+        <v>8</v>
+      </c>
+      <c r="F18" s="9">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G18" s="9">
+        <v>4.4398299999999996E-3</v>
+      </c>
+      <c r="H18" s="9">
+        <v>4.4398299999999996E-3</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>364</v>
+      </c>
+      <c r="J18" s="9"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="9">
+        <v>298</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>1436</v>
+      </c>
+      <c r="D19" s="9">
+        <v>4.9678127700000001</v>
+      </c>
+      <c r="E19" s="9">
+        <v>6</v>
+      </c>
+      <c r="F19" s="9">
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="G19" s="9">
+        <v>1.8663880000000001E-2</v>
+      </c>
+      <c r="H19" s="9">
+        <v>4.7346409999999998E-2</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>1437</v>
+      </c>
+      <c r="J19" s="9" t="s">
+        <v>1438</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="9">
+        <v>247</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>1193</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>1194</v>
+      </c>
+      <c r="D20" s="9">
+        <v>4.8557568499999997</v>
+      </c>
+      <c r="E20" s="9">
+        <v>10</v>
+      </c>
+      <c r="F20" s="9">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="G20" s="9">
+        <v>1.9627500000000001E-3</v>
+      </c>
+      <c r="H20" s="9">
+        <v>8.8767399999999993E-3</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>1195</v>
+      </c>
+      <c r="J20" s="9" t="s">
+        <v>1196</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="9">
+        <v>174</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>863</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>864</v>
+      </c>
+      <c r="D21" s="9">
+        <v>4.6129689999999997</v>
+      </c>
+      <c r="E21" s="9">
+        <v>10</v>
+      </c>
+      <c r="F21" s="9">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G21" s="9">
+        <v>3.025477E-2</v>
+      </c>
+      <c r="H21" s="9">
+        <v>3.5243099999999999E-2</v>
+      </c>
+      <c r="I21" s="9" t="s">
+        <v>865</v>
+      </c>
+      <c r="J21" s="9" t="s">
+        <v>866</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3C0DA80-5772-7D46-84DC-B2ED21FC6016}">
+  <dimension ref="A1:L21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="84.83203125" style="13" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="15"/>
+      <c r="B1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="10">
+        <v>93</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>505</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>506</v>
+      </c>
+      <c r="D2" s="10">
+        <v>12.182014001077</v>
+      </c>
+      <c r="E2" s="10">
+        <v>10</v>
+      </c>
+      <c r="F2" s="10">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G2" s="10">
+        <v>1.9506265794245301E-4</v>
+      </c>
+      <c r="H2" s="10">
+        <v>3.31183385437561E-2</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>504</v>
+      </c>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10">
+        <v>1.9506265794245301E-4</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="10">
+        <v>94</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>507</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>508</v>
+      </c>
+      <c r="D3" s="10">
+        <v>12.182014001077</v>
+      </c>
+      <c r="E3" s="10">
+        <v>10</v>
+      </c>
+      <c r="F3" s="10">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G3" s="10">
+        <v>1.9506265794245301E-4</v>
+      </c>
+      <c r="H3" s="10">
+        <v>3.31183385437561E-2</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>504</v>
+      </c>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10">
+        <v>1.9506265794245301E-4</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="10">
+        <v>239</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>1166</v>
+      </c>
+      <c r="D4" s="10">
+        <v>11.420638126009701</v>
+      </c>
+      <c r="E4" s="10">
+        <v>10</v>
+      </c>
+      <c r="F4" s="10">
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="G4" s="10">
+        <v>1.7934742786836501E-4</v>
+      </c>
+      <c r="H4" s="10">
+        <v>1.08636726407958E-2</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>1167</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>801</v>
+      </c>
+      <c r="K4" s="10">
+        <v>1.7934742786836501E-4</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="10">
+        <v>160</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>799</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>800</v>
+      </c>
+      <c r="D5" s="10">
+        <v>10.9638126009693</v>
+      </c>
+      <c r="E5" s="10">
+        <v>7</v>
+      </c>
+      <c r="F5" s="10">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G5" s="10">
+        <v>4.9963117570514396E-3</v>
+      </c>
+      <c r="H5" s="10">
+        <v>5.7885275829484498E-3</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>758</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>801</v>
+      </c>
+      <c r="K5" s="10">
+        <v>4.9963117570514396E-3</v>
+      </c>
+      <c r="L5" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="10">
+        <v>305</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>1465</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>1466</v>
+      </c>
+      <c r="D6" s="10">
+        <v>10.9638126009693</v>
+      </c>
+      <c r="E6" s="10">
+        <v>10</v>
+      </c>
+      <c r="F6" s="10">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>1467</v>
+      </c>
+      <c r="H6" s="10">
+        <v>1.6656302882084601E-2</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>1167</v>
+      </c>
+      <c r="J6" s="10"/>
+      <c r="K6" s="11" t="s">
+        <v>1468</v>
+      </c>
+      <c r="L6" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="10">
+        <v>321</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>1524</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>1525</v>
+      </c>
+      <c r="D7" s="10">
+        <v>10.9638126009693</v>
+      </c>
+      <c r="E7" s="10">
+        <v>8</v>
+      </c>
+      <c r="F7" s="10">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G7" s="10">
+        <v>1.76127338351206E-3</v>
+      </c>
+      <c r="H7" s="10">
+        <v>3.0100396027309101E-2</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>1526</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>1527</v>
+      </c>
+      <c r="K7" s="10">
+        <v>1.76127338351206E-3</v>
+      </c>
+      <c r="L7" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" s="10">
+        <v>286</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>1384</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>1385</v>
+      </c>
+      <c r="D8" s="10">
+        <v>10.659262250942399</v>
+      </c>
+      <c r="E8" s="10">
+        <v>10</v>
+      </c>
+      <c r="F8" s="10">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>1386</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>1031</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>1387</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>1388</v>
+      </c>
+      <c r="K8" s="11" t="s">
+        <v>1386</v>
+      </c>
+      <c r="L8" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" s="10">
+        <v>92</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>502</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>503</v>
+      </c>
+      <c r="D9" s="10">
+        <v>10.441726286637399</v>
+      </c>
+      <c r="E9" s="10">
+        <v>8</v>
+      </c>
+      <c r="F9" s="10">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G9" s="10">
+        <v>3.4102011929054699E-4</v>
+      </c>
+      <c r="H9" s="10">
+        <v>2.64138216602594E-2</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>504</v>
+      </c>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10">
+        <v>3.4102011929054802E-4</v>
+      </c>
+      <c r="L9" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" s="10">
+        <v>76</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>415</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>416</v>
+      </c>
+      <c r="D10" s="10">
+        <v>9.1365105008077592</v>
+      </c>
+      <c r="E10" s="10">
+        <v>9</v>
+      </c>
+      <c r="F10" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="G10" s="10">
+        <v>6.2343823399003105E-4</v>
+      </c>
+      <c r="H10" s="10">
+        <v>3.8017056899195198E-2</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>417</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>418</v>
+      </c>
+      <c r="K10" s="10">
+        <v>6.2343823399003105E-4</v>
+      </c>
+      <c r="L10" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" s="10">
+        <v>184</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>906</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>907</v>
+      </c>
+      <c r="D11" s="10">
+        <v>9.1365105008077592</v>
+      </c>
+      <c r="E11" s="10">
+        <v>10</v>
+      </c>
+      <c r="F11" s="10">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="G11" s="10">
+        <v>1.41550969110565E-3</v>
+      </c>
+      <c r="H11" s="10">
+        <v>2.5938533693604202E-2</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>908</v>
+      </c>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10">
+        <v>1.41550969110565E-3</v>
+      </c>
+      <c r="L11" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" s="10">
+        <v>203</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>1008</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>1009</v>
+      </c>
+      <c r="D12" s="10">
+        <v>9.1365105008077592</v>
+      </c>
+      <c r="E12" s="10">
+        <v>10</v>
+      </c>
+      <c r="F12" s="10">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="G12" s="10">
+        <v>3.05878163512454E-4</v>
+      </c>
+      <c r="H12" s="10">
+        <v>4.5467445971468998E-3</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>1010</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>1011</v>
+      </c>
+      <c r="K12" s="10">
+        <v>3.05878163512454E-4</v>
+      </c>
+      <c r="L12" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" s="10">
+        <v>270</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>1313</v>
+      </c>
+      <c r="D13" s="10">
+        <v>8.1213426673846705</v>
+      </c>
+      <c r="E13" s="10">
+        <v>10</v>
+      </c>
+      <c r="F13" s="10">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>1314</v>
+      </c>
+      <c r="H13" s="10">
+        <v>1.6017496821703E-3</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>1167</v>
+      </c>
+      <c r="J13" s="10" t="s">
+        <v>634</v>
+      </c>
+      <c r="K13" s="11" t="s">
+        <v>1314</v>
+      </c>
+      <c r="L13" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" s="10">
+        <v>148</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>743</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>744</v>
+      </c>
+      <c r="D14" s="10">
+        <v>7.8312947149780703</v>
+      </c>
+      <c r="E14" s="10">
+        <v>10</v>
+      </c>
+      <c r="F14" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="G14" s="10">
+        <v>2.4722151837369799E-3</v>
+      </c>
+      <c r="H14" s="10">
+        <v>3.1930852281499597E-2</v>
+      </c>
+      <c r="I14" s="10" t="s">
+        <v>745</v>
+      </c>
+      <c r="J14" s="10" t="s">
+        <v>746</v>
+      </c>
+      <c r="K14" s="10">
+        <v>2.4722151837369799E-3</v>
+      </c>
+      <c r="L14" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" s="10">
+        <v>153</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>763</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>764</v>
+      </c>
+      <c r="D15" s="10">
+        <v>7.8312947149780703</v>
+      </c>
+      <c r="E15" s="10">
+        <v>10</v>
+      </c>
+      <c r="F15" s="10">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="G15" s="10">
+        <v>2.2411590660983498E-3</v>
+      </c>
+      <c r="H15" s="10">
+        <v>1.7351748497455799E-2</v>
+      </c>
+      <c r="I15" s="10" t="s">
+        <v>765</v>
+      </c>
+      <c r="J15" s="10" t="s">
+        <v>766</v>
+      </c>
+      <c r="K15" s="10">
+        <v>2.2411590660983498E-3</v>
+      </c>
+      <c r="L15" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" s="10">
+        <v>168</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>835</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>836</v>
+      </c>
+      <c r="D16" s="10">
+        <v>7.8312947149780703</v>
+      </c>
+      <c r="E16" s="10">
+        <v>10</v>
+      </c>
+      <c r="F16" s="10">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>837</v>
+      </c>
+      <c r="H16" s="10">
+        <v>1.9742113317538601E-4</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>838</v>
+      </c>
+      <c r="J16" s="10" t="s">
+        <v>839</v>
+      </c>
+      <c r="K16" s="11" t="s">
+        <v>837</v>
+      </c>
+      <c r="L16" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A17" s="10">
+        <v>259</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>1257</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>1258</v>
+      </c>
+      <c r="D17" s="10">
+        <v>7.3092084006461997</v>
+      </c>
+      <c r="E17" s="10">
+        <v>10</v>
+      </c>
+      <c r="F17" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="G17" s="10">
+        <v>5.7711772687302799E-3</v>
+      </c>
+      <c r="H17" s="10">
+        <v>3.9839748188947303E-2</v>
+      </c>
+      <c r="I17" s="10" t="s">
+        <v>1259</v>
+      </c>
+      <c r="J17" s="10" t="s">
+        <v>1260</v>
+      </c>
+      <c r="K17" s="10">
+        <v>5.7711772687302799E-3</v>
+      </c>
+      <c r="L17" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A18" s="10">
+        <v>257</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>1246</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>1247</v>
+      </c>
+      <c r="D18" s="10">
+        <v>6.9611508577582901</v>
+      </c>
+      <c r="E18" s="10">
+        <v>10</v>
+      </c>
+      <c r="F18" s="10">
+        <v>0.04</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>1248</v>
+      </c>
+      <c r="H18" s="10">
+        <v>2.0226110130846099E-3</v>
+      </c>
+      <c r="I18" s="10" t="s">
+        <v>1249</v>
+      </c>
+      <c r="J18" s="10" t="s">
+        <v>1250</v>
+      </c>
+      <c r="K18" s="11" t="s">
+        <v>1248</v>
+      </c>
+      <c r="L18" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A19" s="10">
+        <v>17</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="D19" s="10">
+        <v>6.8523828756058203</v>
+      </c>
+      <c r="E19" s="10">
+        <v>8</v>
+      </c>
+      <c r="F19" s="10">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G19" s="10">
+        <v>1.39917330503368E-2</v>
+      </c>
+      <c r="H19" s="10">
+        <v>3.8853346683334102E-2</v>
+      </c>
+      <c r="I19" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="J19" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="K19" s="10">
+        <v>1.39917330503368E-2</v>
+      </c>
+      <c r="L19" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A20" s="10">
+        <v>101</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>533</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>534</v>
+      </c>
+      <c r="D20" s="10">
+        <v>6.8523828756058203</v>
+      </c>
+      <c r="E20" s="10">
+        <v>9</v>
+      </c>
+      <c r="F20" s="10">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G20" s="10">
+        <v>9.7829325086427402E-3</v>
+      </c>
+      <c r="H20" s="10">
+        <v>3.9388845697973997E-2</v>
+      </c>
+      <c r="I20" s="10" t="s">
+        <v>535</v>
+      </c>
+      <c r="J20" s="10" t="s">
+        <v>536</v>
+      </c>
+      <c r="K20" s="10">
+        <v>9.7829325086427402E-3</v>
+      </c>
+      <c r="L20" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A21" s="10">
+        <v>217</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>1066</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>1067</v>
+      </c>
+      <c r="D21" s="10">
+        <v>6.5260789291484</v>
+      </c>
+      <c r="E21" s="10">
+        <v>10</v>
+      </c>
+      <c r="F21" s="10">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="G21" s="10">
+        <v>5.6714615027162005E-4</v>
+      </c>
+      <c r="H21" s="10">
+        <v>2.53553493609644E-2</v>
+      </c>
+      <c r="I21" s="10" t="s">
+        <v>1068</v>
+      </c>
+      <c r="J21" s="10" t="s">
+        <v>1069</v>
+      </c>
+      <c r="K21" s="10">
+        <v>5.6714615027162005E-4</v>
+      </c>
+      <c r="L21" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>